<commit_message>
Completed link travel time and path computation slides.
</commit_message>
<xml_diff>
--- a/Manuscript/figures/travel times.xlsx
+++ b/Manuscript/figures/travel times.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emrich\workspace\_2014_UncertainRoadNetworks\PVLDB14_submit\figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad\git\RoadNetworks\Manuscript\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="13275" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="13275"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -109,7 +108,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -127,7 +126,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -802,11 +801,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="63"/>
-        <c:axId val="266348896"/>
-        <c:axId val="266349456"/>
+        <c:axId val="205923296"/>
+        <c:axId val="205923680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="266348896"/>
+        <c:axId val="205923296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,10 +845,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="266349456"/>
+        <c:crossAx val="205923680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -858,7 +857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="266349456"/>
+        <c:axId val="205923680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,10 +905,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="266348896"/>
+        <c:crossAx val="205923296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -962,7 +961,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -992,7 +991,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1007,7 +1006,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1045,7 +1044,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1228,11 +1227,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="328997488"/>
-        <c:axId val="328992448"/>
+        <c:axId val="205991192"/>
+        <c:axId val="205792472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="328997488"/>
+        <c:axId val="205991192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1271,10 +1270,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328992448"/>
+        <c:crossAx val="205792472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1282,7 +1281,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="328992448"/>
+        <c:axId val="205792472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1330,10 +1329,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328997488"/>
+        <c:crossAx val="205991192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1371,7 +1370,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1385,7 +1384,642 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20231725023733735"/>
+          <c:y val="5.4146255911350243E-2"/>
+          <c:w val="0.74759926285810019"/>
+          <c:h val="0.73806997765699001"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Route A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$2:$B$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>7.3864140198966796E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2010166274348706E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8993310039662405E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.921383415594757E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3703148489515828E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3587705844029944E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.9984944188646766E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2385193926498847E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6579523132124786E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1586265944315293E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7335012445998941E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3666447592343149E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0328454086523899E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.6985312568383765E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.3241334253725375E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.867755446071659E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.2897204615498872E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.5573286016989987E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.6490380066905455E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.5573286016989987E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.2897204615498872E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.867755446071659E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.3241334253725375E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.6985312568383765E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.0328454086523899E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.3666447592343149E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.7335012445998941E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.1586265944315293E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.6579523132124786E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.2385193926498847E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.9984944188646766E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.3587705844029944E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.3703148489515828E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.921383415594757E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.8993310039662405E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.2010166274348706E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.3864140198966796E-4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.4182932573835049E-4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.5704649938185112E-4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.4544711584096003E-4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8.0045108603470045E-5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.2845059177051098E-5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.2305037627480895E-5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.1293834981469627E-5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.5618103992730614E-6</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.663956851150913E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="205495184"/>
+        <c:axId val="205494792"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="205495184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
+                  <a:t>Travel</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
+                  <a:t> Time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="205494792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="5"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="205494792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="1"/>
+                  <a:t>Probability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="205495184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2036,8 +2670,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="326033568"/>
-        <c:axId val="326034688"/>
+        <c:axId val="206060632"/>
+        <c:axId val="206070128"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3236,11 +3870,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="326033568"/>
-        <c:axId val="326034688"/>
+        <c:axId val="206060632"/>
+        <c:axId val="206070128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="326033568"/>
+        <c:axId val="206060632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3280,10 +3914,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326034688"/>
+        <c:crossAx val="206070128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3292,7 +3926,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="326034688"/>
+        <c:axId val="206070128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3341,10 +3975,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326033568"/>
+        <c:crossAx val="206060632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3397,7 +4031,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3427,7 +4061,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:userShapes r:id="rId3"/>
@@ -3554,6 +4188,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4574,7 +5248,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4682,11 +5356,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -4697,11 +5366,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -4733,9 +5397,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5089,11 +5750,527 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="51" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5134,15 +6311,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5157,6 +6334,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5308,7 +6515,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9295827" cy="6008628"/>
+    <xdr:ext cx="8647206" cy="6275294"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -5475,7 +6682,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007-2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5483,34 +6690,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -5737,11 +6944,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C47"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -6404,7 +7611,7 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">

</xml_diff>